<commit_message>
Add cover cap to parts list
</commit_message>
<xml_diff>
--- a/SolarTracker_parts_list.xlsx
+++ b/SolarTracker_parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\playground\solar-tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B204F62-5A67-4833-9274-D8B9E3C5267D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBC4F4B-06A3-4428-8749-F405856AC179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="810" windowWidth="28020" windowHeight="14520" xr2:uid="{7A9771AA-6127-456E-A0E1-3EAD2A1E0370}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Arduino Nano</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Example Order</t>
-  </si>
-  <si>
     <t>3D printed parts from the STL directory</t>
   </si>
   <si>
@@ -201,6 +198,15 @@
   </si>
   <si>
     <t>https://www.amazon.de/dp/B0C5H7S96Y?ref=ppx_yo2ov_dt_b_fed_asin_title</t>
+  </si>
+  <si>
+    <t>cover cap of Rituals of Hammam</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/RITUALS-Duschschaum-Vorteilspaket-Das-Ritual-Hammam/dp/B0CL4SBDPQ/ref=asc_df_B0CL4SBDPQ/?tag=googshopde-21&amp;linkCode=df0&amp;hvadid=696322103951&amp;hvpos=&amp;hvnetw=g&amp;hvrand=14682189934117811704&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9042332&amp;hvtargid=pla-2246768438588&amp;psc=1&amp;mcid=87c684332cef3a189cf8231dafe02054&amp;th=1&amp;psc=1&amp;gad_source=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example Order </t>
   </si>
 </sst>
 </file>
@@ -575,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5DD405-F3E3-4D8A-9067-2190345A7F0E}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +602,7 @@
         <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,7 +851,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25">
         <v>10</v>
@@ -861,32 +867,43 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>54</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -913,8 +930,9 @@
     <hyperlink ref="C19" r:id="rId20" display="https://de.aliexpress.com/item/1005007342760815.html?spm=a2g0o.productlist.main.19.8290548buKZp2j&amp;algo_pvid=2665e315-0bdc-497d-ac1c-6180fc65717a&amp;algo_exp_id=2665e315-0bdc-497d-ac1c-6180fc65717a-9&amp;pdp_npi=4%40dis%21EUR%2111.59%2111.59%21%21%2112.54%2112.54%21%40211b61ae17255282949685610e5b54%2112000040344383940%21sea%21DE%212020925812%21X&amp;curPageLogUid=6H1ooLCL51IP&amp;utparam-url=scene%3Asearch%7Cquery_from%3A" xr:uid="{79EEDA9E-A022-425E-A790-A6D6AD3CD67E}"/>
     <hyperlink ref="C20" r:id="rId21" display="https://de.aliexpress.com/item/1005006359548769.html?spm=a2g0o.productlist.main.15.781d33b4PRJB8j&amp;algo_pvid=10dd28cb-bcc4-4cff-a726-af5fd651c5c6&amp;algo_exp_id=10dd28cb-bcc4-4cff-a726-af5fd651c5c6-7&amp;pdp_npi=4%40dis%21EUR%217.34%214.99%21%21%217.94%215.40%21%40211b61ae17255283622836986e5b54%2112000036884070756%21sea%21DE%212020925812%21X&amp;curPageLogUid=JmqEzMTvCoI4&amp;utparam-url=scene%3Asearch%7Cquery_from%3A" xr:uid="{104F832B-DBD9-47BA-9D8F-51E9F8F85AD9}"/>
     <hyperlink ref="C21" r:id="rId22" display="https://de.aliexpress.com/item/1005005478220120.html?spm=a2g0o.productlist.main.3.fa6e26ffxB2dYJ&amp;algo_pvid=c277b967-83e5-421e-b7b6-24ddb521c2e2&amp;algo_exp_id=c277b967-83e5-421e-b7b6-24ddb521c2e2-1&amp;pdp_npi=4%40dis%21EUR%2125.98%2112.99%21%21%21199.54%2199.77%21%40211b61ae17255287970961230e5b54%2112000033243882554%21sea%21DE%212020925812%21X&amp;curPageLogUid=7Mf9owgHCg4j&amp;utparam-url=scene%3Asearch%7Cquery_from%3A" xr:uid="{FC4367CB-DBB1-4F4B-A262-11C429ECF842}"/>
+    <hyperlink ref="C30" r:id="rId23" display="https://www.amazon.de/RITUALS-Duschschaum-Vorteilspaket-Das-Ritual-Hammam/dp/B0CL4SBDPQ/ref=asc_df_B0CL4SBDPQ/?tag=googshopde-21&amp;linkCode=df0&amp;hvadid=696322103951&amp;hvpos=&amp;hvnetw=g&amp;hvrand=14682189934117811704&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9042332&amp;hvtargid=pla-2246768438588&amp;psc=1&amp;mcid=87c684332cef3a189cf8231dafe02054&amp;th=1&amp;psc=1&amp;gad_source=1" xr:uid="{CD226FAF-5D78-4ABE-93B9-8913700A8729}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>